<commit_message>
modified for postgres sql uploading
</commit_message>
<xml_diff>
--- a/data_files/ExportExcel.xlsx
+++ b/data_files/ExportExcel.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EXPLORE\git_files\streamlit_python\data_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC273EFF-BF41-4831-8831-EEA78B1E396C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="381">
   <si>
     <t>ID</t>
   </si>
@@ -912,7 +922,7 @@
     <t>76</t>
   </si>
   <si>
-    <t xml:space="preserve">Investment  Advisor</t>
+    <t>Investment  Advisor</t>
   </si>
   <si>
     <t>Mark_Booth4047@gompie.com</t>
@@ -1153,17 +1163,13 @@
   </si>
   <si>
     <t>Melinda Hancock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data generated with OnlineDataGenerator available at: https://www.onlinedatagenerator.com </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1181,11 +1187,11 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD3D3D3" tint="0"/>
+        <fgColor rgb="FFD3D3D3"/>
       </patternFill>
     </fill>
   </fills>
@@ -1202,35 +1208,340 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:XFD102"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.43" customWidth="1"/>
-    <col min="2" max="2" width="14.43" customWidth="1"/>
-    <col min="3" max="3" width="14.9792261123657" customWidth="1"/>
-    <col min="4" max="4" width="20.8655700683594" customWidth="1"/>
-    <col min="5" max="5" width="14.43" customWidth="1"/>
+    <col min="1" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1247,1712 +1558,1708 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" t="s">
         <v>94</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" t="s">
         <v>101</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>118</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>119</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>120</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>127</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>128</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" t="s">
         <v>129</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" t="s">
         <v>131</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" t="s">
         <v>147</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" t="s">
         <v>148</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" t="s">
         <v>125</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" t="s">
         <v>150</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>152</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" t="s">
         <v>153</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" t="s">
         <v>154</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" t="s">
         <v>155</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" t="s">
         <v>159</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" t="s">
         <v>161</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" t="s">
         <v>165</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" t="s">
         <v>166</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" t="s">
         <v>168</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" t="s">
         <v>169</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" t="s">
         <v>170</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" t="s">
         <v>173</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" t="s">
         <v>174</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" t="s">
         <v>175</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>176</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" t="s">
         <v>177</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" t="s">
         <v>178</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>179</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" t="s">
         <v>173</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" t="s">
         <v>180</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" t="s">
         <v>181</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>182</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" t="s">
         <v>183</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" t="s">
         <v>184</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" t="s">
         <v>125</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" t="s">
         <v>186</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" t="s">
         <v>187</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>188</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" t="s">
         <v>189</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" t="s">
         <v>190</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" t="s">
         <v>191</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>192</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>173</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" t="s">
         <v>193</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" t="s">
         <v>194</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>195</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" t="s">
         <v>196</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" t="s">
         <v>197</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>198</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" t="s">
         <v>199</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" t="s">
         <v>200</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" t="s">
         <v>201</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>202</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" t="s">
         <v>203</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" t="s">
         <v>204</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" t="s">
         <v>205</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>206</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" t="s">
         <v>207</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" t="s">
         <v>208</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>209</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" t="s">
         <v>210</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" t="s">
         <v>211</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" t="s">
         <v>212</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>213</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" t="s">
         <v>203</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" t="s">
         <v>214</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" t="s">
         <v>215</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>216</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" t="s">
         <v>96</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" t="s">
         <v>217</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" t="s">
         <v>218</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>219</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" t="s">
         <v>59</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" t="s">
         <v>220</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" t="s">
         <v>221</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>222</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" t="s">
         <v>189</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" t="s">
         <v>223</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" t="s">
         <v>224</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>225</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" t="s">
         <v>226</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" t="s">
         <v>227</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" t="s">
         <v>228</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>229</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" t="s">
         <v>230</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" t="s">
         <v>231</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>232</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" t="s">
         <v>233</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" t="s">
         <v>234</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" t="s">
         <v>235</v>
       </c>
-      <c r="E58" s="0" t="s">
+      <c r="E58" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>236</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" t="s">
         <v>237</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" t="s">
         <v>238</v>
       </c>
-      <c r="E59" s="0" t="s">
+      <c r="E59" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>240</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" t="s">
         <v>241</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" t="s">
         <v>242</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>243</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" t="s">
         <v>244</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" t="s">
         <v>245</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E61" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>246</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" t="s">
         <v>247</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" t="s">
         <v>248</v>
       </c>
-      <c r="E62" s="0" t="s">
+      <c r="E62" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>249</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" t="s">
         <v>250</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" t="s">
         <v>251</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>252</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" t="s">
         <v>253</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" t="s">
         <v>254</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" t="s">
         <v>255</v>
       </c>
-      <c r="E64" s="0" t="s">
+      <c r="E64" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>257</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" t="s">
         <v>118</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" t="s">
         <v>258</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" t="s">
         <v>259</v>
       </c>
-      <c r="E65" s="0" t="s">
+      <c r="E65" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>261</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" t="s">
         <v>96</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" t="s">
         <v>262</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" t="s">
         <v>263</v>
       </c>
-      <c r="E66" s="0" t="s">
+      <c r="E66" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>264</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" t="s">
         <v>265</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" t="s">
         <v>266</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" t="s">
         <v>267</v>
       </c>
-      <c r="E67" s="0" t="s">
+      <c r="E67" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>268</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" t="s">
         <v>269</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" t="s">
         <v>270</v>
       </c>
-      <c r="D68" s="0" t="s">
+      <c r="D68" t="s">
         <v>271</v>
       </c>
-      <c r="E68" s="0" t="s">
+      <c r="E68" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>273</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" t="s">
         <v>146</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" t="s">
         <v>274</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" t="s">
         <v>275</v>
       </c>
-      <c r="E69" s="0" t="s">
+      <c r="E69" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>276</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" t="s">
         <v>277</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" t="s">
         <v>278</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>279</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" t="s">
         <v>74</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" t="s">
         <v>280</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" t="s">
         <v>281</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E71" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>282</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" t="s">
         <v>283</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" t="s">
         <v>284</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="E72" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>285</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" t="s">
         <v>286</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" t="s">
         <v>287</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" t="s">
         <v>288</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>289</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" t="s">
         <v>290</v>
       </c>
-      <c r="D74" s="0" t="s">
+      <c r="D74" t="s">
         <v>291</v>
       </c>
-      <c r="E74" s="0" t="s">
+      <c r="E74" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>292</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" t="s">
         <v>293</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" t="s">
         <v>294</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" t="s">
         <v>295</v>
       </c>
-      <c r="E75" s="0" t="s">
+      <c r="E75" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>296</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" t="s">
         <v>118</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" t="s">
         <v>297</v>
       </c>
-      <c r="D76" s="0" t="s">
+      <c r="D76" t="s">
         <v>298</v>
       </c>
-      <c r="E76" s="0" t="s">
+      <c r="E76" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>299</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" t="s">
         <v>300</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" t="s">
         <v>301</v>
       </c>
-      <c r="D77" s="0" t="s">
+      <c r="D77" t="s">
         <v>302</v>
       </c>
-      <c r="E77" s="0" t="s">
+      <c r="E77" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>303</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" t="s">
         <v>189</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" t="s">
         <v>304</v>
       </c>
-      <c r="D78" s="0" t="s">
+      <c r="D78" t="s">
         <v>305</v>
       </c>
-      <c r="E78" s="0" t="s">
+      <c r="E78" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>306</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" t="s">
         <v>307</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" t="s">
         <v>308</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" t="s">
         <v>309</v>
       </c>
-      <c r="E79" s="0" t="s">
+      <c r="E79" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>310</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" t="s">
         <v>31</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C80" t="s">
         <v>311</v>
       </c>
-      <c r="D80" s="0" t="s">
+      <c r="D80" t="s">
         <v>312</v>
       </c>
-      <c r="E80" s="0" t="s">
+      <c r="E80" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>313</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" t="s">
         <v>64</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C81" t="s">
         <v>314</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D81" t="s">
         <v>315</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E81" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>316</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" t="s">
         <v>317</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" t="s">
         <v>318</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="D82" t="s">
         <v>319</v>
       </c>
-      <c r="E82" s="0" t="s">
+      <c r="E82" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="0" t="s">
+    <row r="83" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>320</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" t="s">
         <v>79</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" t="s">
         <v>321</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="D83" t="s">
         <v>322</v>
       </c>
-      <c r="E83" s="0" t="s">
+      <c r="E83" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="0" t="s">
+    <row r="84" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>323</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" t="s">
         <v>324</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" t="s">
         <v>325</v>
       </c>
-      <c r="D84" s="0" t="s">
+      <c r="D84" t="s">
         <v>326</v>
       </c>
-      <c r="E84" s="0" t="s">
+      <c r="E84" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="0" t="s">
+    <row r="85" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>327</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" t="s">
         <v>269</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" t="s">
         <v>328</v>
       </c>
-      <c r="D85" s="0" t="s">
+      <c r="D85" t="s">
         <v>329</v>
       </c>
-      <c r="E85" s="0" t="s">
+      <c r="E85" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="0" t="s">
+    <row r="86" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>330</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="C86" t="s">
         <v>331</v>
       </c>
-      <c r="D86" s="0" t="s">
+      <c r="D86" t="s">
         <v>332</v>
       </c>
-      <c r="E86" s="0" t="s">
+      <c r="E86" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="0" t="s">
+    <row r="87" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>333</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" t="s">
         <v>334</v>
       </c>
-      <c r="C87" s="0" t="s">
+      <c r="C87" t="s">
         <v>335</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="D87" t="s">
         <v>336</v>
       </c>
-      <c r="E87" s="0" t="s">
+      <c r="E87" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="0" t="s">
+    <row r="88" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>337</v>
       </c>
-      <c r="B88" s="0" t="s">
+      <c r="B88" t="s">
         <v>64</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" t="s">
         <v>338</v>
       </c>
-      <c r="D88" s="0" t="s">
+      <c r="D88" t="s">
         <v>339</v>
       </c>
-      <c r="E88" s="0" t="s">
+      <c r="E88" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="0" t="s">
+    <row r="89" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>340</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B89" t="s">
         <v>324</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" t="s">
         <v>341</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D89" t="s">
         <v>342</v>
       </c>
-      <c r="E89" s="0" t="s">
+      <c r="E89" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="0" t="s">
+    <row r="90" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>343</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" t="s">
         <v>74</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" t="s">
         <v>344</v>
       </c>
-      <c r="D90" s="0" t="s">
+      <c r="D90" t="s">
         <v>345</v>
       </c>
-      <c r="E90" s="0" t="s">
+      <c r="E90" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="0" t="s">
+    <row r="91" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>346</v>
       </c>
-      <c r="B91" s="0" t="s">
+      <c r="B91" t="s">
         <v>146</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C91" t="s">
         <v>347</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D91" t="s">
         <v>348</v>
       </c>
-      <c r="E91" s="0" t="s">
+      <c r="E91" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="0" t="s">
+    <row r="92" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>349</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" t="s">
         <v>350</v>
       </c>
-      <c r="C92" s="0" t="s">
+      <c r="C92" t="s">
         <v>351</v>
       </c>
-      <c r="D92" s="0" t="s">
+      <c r="D92" t="s">
         <v>352</v>
       </c>
-      <c r="E92" s="0" t="s">
+      <c r="E92" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="0" t="s">
+    <row r="93" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>353</v>
       </c>
-      <c r="B93" s="0" t="s">
+      <c r="B93" t="s">
         <v>168</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C93" t="s">
         <v>354</v>
       </c>
-      <c r="D93" s="0" t="s">
+      <c r="D93" t="s">
         <v>355</v>
       </c>
-      <c r="E93" s="0" t="s">
+      <c r="E93" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="0" t="s">
+    <row r="94" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>356</v>
       </c>
-      <c r="B94" s="0" t="s">
+      <c r="B94" t="s">
         <v>173</v>
       </c>
-      <c r="C94" s="0" t="s">
+      <c r="C94" t="s">
         <v>357</v>
       </c>
-      <c r="D94" s="0" t="s">
+      <c r="D94" t="s">
         <v>358</v>
       </c>
-      <c r="E94" s="0" t="s">
+      <c r="E94" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="0" t="s">
+    <row r="95" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>359</v>
       </c>
-      <c r="B95" s="0" t="s">
+      <c r="B95" t="s">
         <v>104</v>
       </c>
-      <c r="C95" s="0" t="s">
+      <c r="C95" t="s">
         <v>360</v>
       </c>
-      <c r="D95" s="0" t="s">
+      <c r="D95" t="s">
         <v>361</v>
       </c>
-      <c r="E95" s="0" t="s">
+      <c r="E95" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="0" t="s">
+    <row r="96" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>362</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" t="s">
         <v>189</v>
       </c>
-      <c r="C96" s="0" t="s">
+      <c r="C96" t="s">
         <v>363</v>
       </c>
-      <c r="D96" s="0" t="s">
+      <c r="D96" t="s">
         <v>364</v>
       </c>
-      <c r="E96" s="0" t="s">
+      <c r="E96" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="0" t="s">
+    <row r="97" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>365</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" t="s">
         <v>134</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="C97" t="s">
         <v>366</v>
       </c>
-      <c r="D97" s="0" t="s">
+      <c r="D97" t="s">
         <v>367</v>
       </c>
-      <c r="E97" s="0" t="s">
+      <c r="E97" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="0" t="s">
+    <row r="98" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>368</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" t="s">
         <v>6</v>
       </c>
-      <c r="C98" s="0" t="s">
+      <c r="C98" t="s">
         <v>369</v>
       </c>
-      <c r="D98" s="0" t="s">
+      <c r="D98" t="s">
         <v>370</v>
       </c>
-      <c r="E98" s="0" t="s">
+      <c r="E98" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="0" t="s">
+    <row r="99" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>371</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" t="s">
         <v>372</v>
       </c>
-      <c r="D99" s="0" t="s">
+      <c r="D99" t="s">
         <v>373</v>
       </c>
-      <c r="E99" s="0" t="s">
+      <c r="E99" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="0" t="s">
+    <row r="100" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>374</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="B100" t="s">
         <v>203</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" t="s">
         <v>375</v>
       </c>
-      <c r="D100" s="0" t="s">
+      <c r="D100" t="s">
         <v>376</v>
       </c>
-      <c r="E100" s="0" t="s">
+      <c r="E100" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="0" t="s">
+    <row r="101" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>378</v>
       </c>
-      <c r="B101" s="0" t="s">
+      <c r="B101" t="s">
         <v>21</v>
       </c>
-      <c r="C101" s="0" t="s">
+      <c r="C101" t="s">
         <v>379</v>
       </c>
-      <c r="D101" s="0" t="s">
+      <c r="D101" t="s">
         <v>380</v>
       </c>
-      <c r="E101" s="0" t="s">
+      <c r="E101" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="0" t="s">
-        <v>381</v>
-      </c>
-    </row>
+    <row r="102" spans="1:5" ht="12.5" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>